<commit_message>
Testing Techniques, System testing and testing types
</commit_message>
<xml_diff>
--- a/ManualTestingTopics.xlsx
+++ b/ManualTestingTopics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarth\Desktop\SOFTWARE TESTING\MANUAL TESTING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarth\Desktop\SOFTWARE TESTING\MANUAL_TESTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF5E0B87-67F7-4E50-969D-931A98EF274D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EB3AFE-956B-4C20-8FE4-096F0AA7A6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11A1106E-0D72-436A-B383-1F515D32D33E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Topics of Discussion</t>
   </si>
@@ -66,16 +66,6 @@
   </si>
   <si>
     <t>9. Different Levels of Software Testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10. White Box 
-       BlackBox
-       Static
-        Dynamic
-       </t>
-  </si>
-  <si>
-    <t>11. Verification and Validation</t>
   </si>
   <si>
     <t>12. System Testing Types</t>
@@ -154,6 +144,22 @@
 V-model vs Waterfall model
 Sprial vs V-Model</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">10. White Box 
+       BlackBox
+       Static
+       Dynamic
+       </t>
+  </si>
+  <si>
+    <t>11. Verification vs Validation</t>
+  </si>
+  <si>
+    <t>Negative and Positive Testing</t>
+  </si>
+  <si>
+    <t>Globalization and Localization Testing</t>
   </si>
 </sst>
 </file>
@@ -561,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BC0177-6806-4B8C-A4CF-8EEF8580A257}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="53.44140625" defaultRowHeight="52.8" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -607,7 +613,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
@@ -626,98 +632,104 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="154.80000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="1" t="s">
+    <row r="14" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="1" t="s">
+    <row r="15" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="1" t="s">
+    <row r="16" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A15" s="1" t="s">
+    <row r="17" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="1" t="s">
+    <row r="18" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A18" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="1" t="s">
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="1" t="s">
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="1" t="s">
+    <row r="22" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="1" t="s">
+    <row r="23" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="1" t="s">
+    <row r="24" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="1" t="s">
+    <row r="25" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="1" t="s">
+    <row r="26" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="1" t="s">
+    <row r="27" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A26" s="1" t="s">
+    <row r="28" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A27" s="1" t="s">
+    <row r="29" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="1" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A29" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding Test Case Document
</commit_message>
<xml_diff>
--- a/ManualTestingTopics.xlsx
+++ b/ManualTestingTopics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarth\Desktop\SOFTWARE TESTING\MANUAL_TESTING\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarth\Desktop\SOFTWARE TESTING\May_2023_WeekDay_Batch\MANUAL_TESTING\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EB3AFE-956B-4C20-8FE4-096F0AA7A6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F96FD6-134E-4EFD-93B9-020AD0C2F6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{11A1106E-0D72-436A-B383-1F515D32D33E}"/>
   </bookViews>
@@ -627,7 +627,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
@@ -688,27 +688,27 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="52.8" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="4" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>